<commit_message>
fixing axis labels other minor changes
</commit_message>
<xml_diff>
--- a/zqlparserdemo/zqlexamples.xlsx
+++ b/zqlparserdemo/zqlexamples.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eideh\Documents\GitHub\zenvisage\zqlparserdemo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="10523" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23880" windowHeight="14040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -199,24 +199,18 @@
   </si>
   <si>
     <t>state='NY'</t>
-  </si>
-  <si>
-    <t>^ this query does not work right now, since we are just ANDING constraints. We will get nothing if we and state='CA' and state='NY'</t>
-  </si>
-  <si>
-    <t>^ works perfectly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -343,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -365,23 +359,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -707,21 +690,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="18.6875" customWidth="1"/>
-    <col min="3" max="3" width="33.1875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="6" width="21.6875" customWidth="1"/>
-    <col min="7" max="7" width="50.75" customWidth="1"/>
-    <col min="8" max="8" width="5.6875" customWidth="1"/>
-    <col min="9" max="9" width="74.6875" customWidth="1"/>
+    <col min="5" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="50.83203125" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" customWidth="1"/>
+    <col min="9" max="9" width="74.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1185,7 +1168,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" ht="24">
       <c r="A39" s="8" t="s">
         <v>31</v>
       </c>
@@ -1206,9 +1189,7 @@
       <c r="A40" s="11"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
-      <c r="D40" s="12" t="s">
-        <v>61</v>
-      </c>
+      <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13"/>
@@ -1272,13 +1253,28 @@
       <c r="F43" s="8"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="1:7" ht="78.75">
-      <c r="E44" s="15" t="s">
-        <v>60</v>
+    <row r="44" spans="1:7" ht="16" thickBot="1"/>
+    <row r="45" spans="1:7" ht="16" thickBot="1">
+      <c r="A45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some query meanings
</commit_message>
<xml_diff>
--- a/zqlparserdemo/zqlexamples.xlsx
+++ b/zqlparserdemo/zqlexamples.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eideh\Documents\GitHub\zenvisage\zqlparserdemo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18920" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18923" windowHeight="14738" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -205,13 +210,22 @@
   </si>
   <si>
     <t>^ works perfectly</t>
+  </si>
+  <si>
+    <t>Meaning:</t>
+  </si>
+  <si>
+    <t>Return top 7 states that have the most similar soldprice over year visualization to CA</t>
+  </si>
+  <si>
+    <t>Returns the visualization for CA and NY (among different combinations of X and Y) that are most similar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -281,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -355,13 +369,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -386,6 +409,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -727,21 +761,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6875" customWidth="1"/>
+    <col min="3" max="3" width="33.1875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="50.6640625" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" customWidth="1"/>
-    <col min="9" max="9" width="74.6640625" customWidth="1"/>
+    <col min="5" max="6" width="21.6875" customWidth="1"/>
+    <col min="7" max="7" width="50.6875" customWidth="1"/>
+    <col min="8" max="8" width="5.6875" customWidth="1"/>
+    <col min="9" max="9" width="74.6875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1106,208 +1140,235 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1"/>
-    <row r="29" spans="1:9">
-      <c r="G29" t="s">
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1"/>
+    <row r="30" spans="1:9">
+      <c r="G30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="G31" t="s">
+    <row r="32" spans="1:9">
+      <c r="G32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="1" customFormat="1"/>
-    <row r="33" spans="1:7">
-      <c r="A33" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="33" spans="1:7" s="1" customFormat="1"/>
     <row r="34" spans="1:7">
       <c r="A34" s="7" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16.149999999999999" thickBot="1">
+      <c r="A36" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D36" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1"/>
     <row r="37" spans="1:7">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+    </row>
+    <row r="38" spans="1:7" s="1" customFormat="1" ht="16.149999999999999" thickBot="1"/>
+    <row r="39" spans="1:7">
+      <c r="A39" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C39" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="8" t="s">
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B40" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C40" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8" t="s">
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="24">
-      <c r="A39" s="8" t="s">
+    <row r="41" spans="1:7" ht="16.149999999999999" thickBot="1">
+      <c r="A41" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B41" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="11"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12" t="s">
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" ht="79.150000000000006" thickBot="1">
+      <c r="A42" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="20"/>
+    </row>
+    <row r="43" spans="1:7" ht="16.149999999999999" thickBot="1">
+      <c r="A43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="13"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="8" t="s">
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C44" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D44" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E44" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="8" t="s">
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B45" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C45" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D45" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8" t="s">
+      <c r="F45" s="8"/>
+      <c r="G45" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="8" t="s">
+    <row r="46" spans="1:7">
+      <c r="A46" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C46" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D46" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="10"/>
-    </row>
-    <row r="44" spans="1:7" ht="73" thickBot="1">
-      <c r="E44" s="15" t="s">
+      <c r="F46" s="8"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" ht="79.150000000000006" thickBot="1">
+      <c r="E47" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="16" thickBot="1">
-      <c r="A45" s="8" t="s">
+    <row r="48" spans="1:7" ht="16.149999999999999" thickBot="1">
+      <c r="A48" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B48" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C48" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed the zqlexamples file Was not correct after merge
</commit_message>
<xml_diff>
--- a/zqlparserdemo/zqlexamples.xlsx
+++ b/zqlparserdemo/zqlexamples.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eideh\Documents\GitHub\zenvisage\zqlparserdemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eideh\Documents\Github\zenvisage\zqlparserdemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18923" windowHeight="14738" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18930" windowHeight="14745" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -769,13 +769,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="18.6875" customWidth="1"/>
-    <col min="3" max="3" width="33.1875" customWidth="1"/>
+    <col min="2" max="2" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="33.25" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="6" width="21.6875" customWidth="1"/>
-    <col min="7" max="7" width="50.6875" customWidth="1"/>
-    <col min="8" max="8" width="5.6875" customWidth="1"/>
-    <col min="9" max="9" width="74.6875" customWidth="1"/>
+    <col min="5" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="7" width="50.75" customWidth="1"/>
+    <col min="8" max="8" width="5.75" customWidth="1"/>
+    <col min="9" max="9" width="74.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1193,7 +1193,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.149999999999999" thickBot="1">
+    <row r="36" spans="1:7" ht="16.5" thickBot="1">
       <c r="A36" s="7" t="s">
         <v>31</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
     </row>
-    <row r="38" spans="1:7" s="1" customFormat="1" ht="16.149999999999999" thickBot="1"/>
+    <row r="38" spans="1:7" s="1" customFormat="1" ht="16.5" thickBot="1"/>
     <row r="39" spans="1:7">
       <c r="A39" s="8" t="s">
         <v>8</v>
@@ -1253,7 +1253,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16.149999999999999" thickBot="1">
+    <row r="41" spans="1:7" ht="16.5" thickBot="1">
       <c r="A41" s="8" t="s">
         <v>31</v>
       </c>
@@ -1270,7 +1270,7 @@
       <c r="F41" s="9"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:7" ht="79.150000000000006" thickBot="1">
+    <row r="42" spans="1:7" ht="81.75" thickBot="1">
       <c r="A42" s="17" t="s">
         <v>62</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="F42" s="19"/>
       <c r="G42" s="20"/>
     </row>
-    <row r="43" spans="1:7" ht="16.149999999999999" thickBot="1">
+    <row r="43" spans="1:7" ht="16.5" thickBot="1">
       <c r="A43" s="11"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -1353,12 +1353,12 @@
       <c r="F46" s="8"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="1:7" ht="79.150000000000006" thickBot="1">
+    <row r="47" spans="1:7" ht="81.75" thickBot="1">
       <c r="E47" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="16.149999999999999" thickBot="1">
+    <row r="48" spans="1:7" ht="16.5" thickBot="1">
       <c r="A48" s="8" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Restored old TIncreasing algorithm
</commit_message>
<xml_diff>
--- a/zqlparserdemo/zqlexamples.xlsx
+++ b/zqlparserdemo/zqlexamples.xlsx
@@ -176,9 +176,6 @@
     <t>y2&lt;-{'listingprice'}</t>
   </si>
   <si>
-    <t>v1&lt;-argmin_{y1,y2}[k=7]DEuclidean(f1,f2)</t>
-  </si>
-  <si>
     <t>y3&lt;-{'soldprice','listingprice'}</t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>Returns the visualization for CA and NY (among different combinations of X and Y) that are most similar</t>
+  </si>
+  <si>
+    <t>v1&lt;-argmin_{z1}[k=7]DEuclidean(f1,f2)</t>
   </si>
 </sst>
 </file>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1142,10 +1142,10 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
         <v>62</v>
-      </c>
-      <c r="B28" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1"/>
@@ -1190,7 +1190,7 @@
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1">
@@ -1201,13 +1201,13 @@
         <v>18</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>32</v>
       </c>
       <c r="E36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1228,7 +1228,7 @@
         <v>25</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
@@ -1245,12 +1245,12 @@
         <v>19</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16.5" thickBot="1">
@@ -1258,13 +1258,13 @@
         <v>31</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -1272,10 +1272,10 @@
     </row>
     <row r="42" spans="1:7" ht="81.75" thickBot="1">
       <c r="A42" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -1288,7 +1288,7 @@
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
@@ -1327,11 +1327,11 @@
         <v>20</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1339,10 +1339,10 @@
         <v>31</v>
       </c>
       <c r="B46" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>20</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="47" spans="1:7" ht="81.75" thickBot="1">
       <c r="E47" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="16.5" thickBot="1">

</xml_diff>